<commit_message>
Working version with transactions exceptions and pretty API. Correct Dashboard. Still lower/errors and request to be revised
</commit_message>
<xml_diff>
--- a/MPL dashboard.xlsx
+++ b/MPL dashboard.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{04593556-0A93-4836-BBA1-96DE7C8057B0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{ABCF0F21-C453-458D-8E17-F47399F55175}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="792" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="792" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phones" sheetId="1" r:id="rId1"/>
@@ -1119,7 +1119,9 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1182,7 +1184,7 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adds all necessary fields
</commit_message>
<xml_diff>
--- a/MPL dashboard.xlsx
+++ b/MPL dashboard.xlsx
@@ -1,32 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{EFBEE222-042D-46D4-B38E-1160A1C14631}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8096B34D-F0EA-462A-BEE5-EE1170B0413C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" tabRatio="792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7680" tabRatio="792" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phones" sheetId="1" r:id="rId1"/>
-    <sheet name="Commitment Discounts" sheetId="3" r:id="rId2"/>
+    <sheet name="Exceptions" sheetId="2" r:id="rId2"/>
     <sheet name="Tariff Discounts" sheetId="4" r:id="rId3"/>
-    <sheet name="Transaction Discounts" sheetId="7" r:id="rId4"/>
-    <sheet name="Channel Discounts" sheetId="6" r:id="rId5"/>
-    <sheet name="Finance Discounts" sheetId="5" r:id="rId6"/>
-    <sheet name="Exceptions" sheetId="2" r:id="rId7"/>
+    <sheet name="Commitment Discounts" sheetId="3" r:id="rId4"/>
+    <sheet name="Transaction Discounts" sheetId="7" r:id="rId5"/>
+    <sheet name="Channel Discounts" sheetId="6" r:id="rId6"/>
+    <sheet name="Finance Discounts" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Model</t>
   </si>
@@ -118,15 +123,6 @@
     <t>Finance_Conditions</t>
   </si>
   <si>
-    <t>Xiaomi</t>
-  </si>
-  <si>
-    <t>Mi8 Lite 4</t>
-  </si>
-  <si>
-    <t>Mid</t>
-  </si>
-  <si>
     <t>Hibrid</t>
   </si>
   <si>
@@ -139,9 +135,6 @@
     <t xml:space="preserve">Neogranicena </t>
   </si>
   <si>
-    <t>Tarifa za mlade</t>
-  </si>
-  <si>
     <t>CP</t>
   </si>
   <si>
@@ -157,7 +150,46 @@
     <t>Credit_Note</t>
   </si>
   <si>
-    <t>Mi8 Lite 4+64</t>
+    <t>iPhone 11</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>iPhone 11 64GB Black</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>MNP</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Hibrid mini</t>
+  </si>
+  <si>
+    <t>64 GB</t>
+  </si>
+  <si>
+    <t>Tariff Name</t>
+  </si>
+  <si>
+    <t>PRP</t>
+  </si>
+  <si>
+    <t>128 GB</t>
+  </si>
+  <si>
+    <t>XXX124</t>
+  </si>
+  <si>
+    <t>Najbolja L</t>
   </si>
 </sst>
 </file>
@@ -233,6 +265,21 @@
   </cellStyles>
   <dxfs count="7">
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -255,21 +302,6 @@
           <bgColor theme="1" tint="0.499984740745262"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -316,14 +348,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FDE4A110-E8BE-4B94-AE3D-673F8588BC62}" name="Table6" displayName="Table6" ref="A1:I2" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="A1:I2" xr:uid="{37D71D34-ECA6-4ECB-8035-17A18198947C}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FDE4A110-E8BE-4B94-AE3D-673F8588BC62}" name="Table6" displayName="Table6" ref="A1:J2" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:J2" xr:uid="{37D71D34-ECA6-4ECB-8035-17A18198947C}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{C4BBC66E-A077-4B9A-81BA-F0CB603496B5}" name="SAPcode"/>
     <tableColumn id="2" xr3:uid="{0CAAE7D9-EE2C-43B5-9DD9-E8205D5B58A5}" name="Name"/>
     <tableColumn id="3" xr3:uid="{AE90FA23-35D6-47C6-A3A7-F063AAE546AB}" name="Manufacturer"/>
     <tableColumn id="4" xr3:uid="{24E75171-FFB3-4F81-9C86-B439AF49DD2B}" name="Model"/>
     <tableColumn id="5" xr3:uid="{A6B405D0-99BF-417B-895A-2BDF363360D1}" name="Memory"/>
+    <tableColumn id="9" xr3:uid="{BB97B1A7-81BE-4DBD-A2C9-A3B9D52DBD7F}" name="Color"/>
     <tableColumn id="6" xr3:uid="{E7149D11-C82B-46A9-9305-2CB35CB385A5}" name="Segment"/>
     <tableColumn id="7" xr3:uid="{AB5070AE-C2C2-46CC-A336-5421DAEF28E4}" name="MAP"/>
     <tableColumn id="10" xr3:uid="{0F31BE27-F96B-484E-A865-E03ECD6046FC}" name="Credit_Note"/>
@@ -334,69 +367,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E0E62921-B196-47B1-9B3E-8B2C3763628D}" name="Table5" displayName="Table5" ref="A1:B4" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A1:B4" xr:uid="{AAFA30A5-D6C7-40E5-9F4D-2E4F86E44CB7}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{941F5ACE-343A-47E0-84A1-BC4B35BC930D}" name="Commitment"/>
-    <tableColumn id="2" xr3:uid="{5C010D87-1024-4813-8703-AC26ECB31BE0}" name="Commitment_Discount"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2AF0536D-D79A-4B7E-AE73-BEBC0D5A9102}" name="Table4" displayName="Table4" ref="A1:B6" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:B6" xr:uid="{E94A05D0-2941-4012-B2D5-96C907A9D8E7}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2206CDE1-E219-4F96-B0D9-89A372AD6A10}" name="Tariff"/>
-    <tableColumn id="2" xr3:uid="{4B83F139-CBC5-4141-A55C-9DC5DE7D0C89}" name="Tariff_Discount"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DDD352F4-F3AE-4479-AA1F-12647518967E}" name="Table38" displayName="Table38" ref="A1:B4" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:B4" xr:uid="{B9A0EF7A-6FF4-44BC-A246-AA3356376106}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D94E6893-4879-4AED-8A01-518D163F8677}" name="Transaction"/>
-    <tableColumn id="2" xr3:uid="{F0E2D9DC-99EC-4AE1-BE98-79D3F5668115}" name="Transaction_Discount"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4591949D-C562-4CC3-AB24-A72046876E21}" name="Table3" displayName="Table3" ref="A1:B6" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:B6" xr:uid="{3F3CC5C3-0F9B-4504-932C-38EEF0ECF058}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{766318BB-F216-40D1-9821-6788E3D1DF19}" name="Channel"/>
-    <tableColumn id="2" xr3:uid="{9B8803A6-592E-4211-93C5-89EF0E354362}" name="Channel_Discount"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4B9CACF-7FE2-4C55-A8CF-BD14747CFCD6}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:B5" xr:uid="{60B68E3F-348B-4138-97F8-FBF9EEEF1350}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{60A8D2BE-6A85-47CC-885D-804FD5E4F5C2}" name="Finance_Conditions"/>
-    <tableColumn id="2" xr3:uid="{B1D4FA89-0886-48EC-BDAD-04C0031891E4}" name="Finance_Discount"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2F026AB0-B205-44B7-BF34-491C2B0292DA}" name="Table1" displayName="Table1" ref="A1:N2" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:N2" xr:uid="{AE85AC31-E6A2-47AF-BABA-3C5B6391840F}"/>
-  <tableColumns count="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2F026AB0-B205-44B7-BF34-491C2B0292DA}" name="Table1" displayName="Table1" ref="A1:O4" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:O4" xr:uid="{AE85AC31-E6A2-47AF-BABA-3C5B6391840F}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{82143DFF-EBA7-4AC4-B7F3-C5FC349EAFD5}" name="SAPcode"/>
     <tableColumn id="2" xr3:uid="{11EAE29A-BFF7-49BF-BD26-C60529EE89F2}" name="Name"/>
     <tableColumn id="3" xr3:uid="{DF952ED5-A765-4D63-AF35-8E70652126F0}" name="Manufacturer"/>
     <tableColumn id="4" xr3:uid="{D6AFD2E0-9343-4063-A311-32534A099952}" name="Model"/>
     <tableColumn id="5" xr3:uid="{5F22A3E3-4D92-40A6-AD12-36271A780C5E}" name="Memory"/>
+    <tableColumn id="15" xr3:uid="{15571AED-EC3C-424B-BD70-A0C960DE46CB}" name="Color"/>
     <tableColumn id="6" xr3:uid="{05EF0420-B340-42F7-9A1C-0487440809AE}" name="Segment"/>
     <tableColumn id="7" xr3:uid="{F94E05DA-EBD5-4535-8965-FB2348E85BD7}" name="Tariff"/>
     <tableColumn id="8" xr3:uid="{C27E7323-6CA7-4662-850F-508035116A4D}" name="Commitment"/>
@@ -406,6 +385,61 @@
     <tableColumn id="11" xr3:uid="{C7625E6A-9C66-471C-8136-65CDEFEBB029}" name="Correction"/>
     <tableColumn id="13" xr3:uid="{F76B42CE-BBA3-4D0D-8AAC-E3AD9882EEBB}" name="from"/>
     <tableColumn id="14" xr3:uid="{057DB79B-4DF3-483D-8187-C242C433CABE}" name="to"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2AF0536D-D79A-4B7E-AE73-BEBC0D5A9102}" name="Table4" displayName="Table4" ref="A1:B7" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:B7" xr:uid="{E94A05D0-2941-4012-B2D5-96C907A9D8E7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{2206CDE1-E219-4F96-B0D9-89A372AD6A10}" name="Tariff Name"/>
+    <tableColumn id="2" xr3:uid="{4B83F139-CBC5-4141-A55C-9DC5DE7D0C89}" name="Tariff_Discount"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E0E62921-B196-47B1-9B3E-8B2C3763628D}" name="Table5" displayName="Table5" ref="A1:B4" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:B4" xr:uid="{AAFA30A5-D6C7-40E5-9F4D-2E4F86E44CB7}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{941F5ACE-343A-47E0-84A1-BC4B35BC930D}" name="Commitment"/>
+    <tableColumn id="2" xr3:uid="{5C010D87-1024-4813-8703-AC26ECB31BE0}" name="Commitment_Discount"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DDD352F4-F3AE-4479-AA1F-12647518967E}" name="Table38" displayName="Table38" ref="A1:B5" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:B5" xr:uid="{B9A0EF7A-6FF4-44BC-A246-AA3356376106}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D94E6893-4879-4AED-8A01-518D163F8677}" name="Transaction"/>
+    <tableColumn id="2" xr3:uid="{F0E2D9DC-99EC-4AE1-BE98-79D3F5668115}" name="Transaction_Discount"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4591949D-C562-4CC3-AB24-A72046876E21}" name="Table3" displayName="Table3" ref="A1:B6" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:B6" xr:uid="{3F3CC5C3-0F9B-4504-932C-38EEF0ECF058}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{766318BB-F216-40D1-9821-6788E3D1DF19}" name="Channel"/>
+    <tableColumn id="2" xr3:uid="{9B8803A6-592E-4211-93C5-89EF0E354362}" name="Channel_Discount"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C4B9CACF-7FE2-4C55-A8CF-BD14747CFCD6}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B5" xr:uid="{60B68E3F-348B-4138-97F8-FBF9EEEF1350}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{60A8D2BE-6A85-47CC-885D-804FD5E4F5C2}" name="Finance_Conditions"/>
+    <tableColumn id="2" xr3:uid="{B1D4FA89-0886-48EC-BDAD-04C0031891E4}" name="Finance_Discount"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -675,12 +709,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
-    <tabColor rgb="FFFF0066"/>
+    <tabColor theme="0" tint="-0.499984740745262"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,13 +723,13 @@
     <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
-    <col min="7" max="8" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="8" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -712,45 +746,83 @@
         <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2">
-        <v>64</v>
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="4">
-        <v>1260</v>
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
       </c>
       <c r="H2" s="4">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>2498</v>
+        <v>4545</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5000</v>
+      </c>
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>6500</v>
       </c>
     </row>
   </sheetData>
@@ -763,6 +835,277 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B22AAE5-670B-4978-B895-98848E155129}">
+  <sheetPr codeName="Sheet6">
+    <tabColor theme="0" tint="-0.499984740745262"/>
+  </sheetPr>
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C068D245-8A86-449D-8532-1989B477943D}">
+          <x14:formula1>
+            <xm:f>'Commitment Discounts'!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1E1ABC66-F73B-477D-A05B-ECEEB0AD15F6}">
+          <x14:formula1>
+            <xm:f>'Channel Discounts'!$A$2:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>J2:J4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{78496895-BF35-4507-A616-3CFF1609171C}">
+          <x14:formula1>
+            <xm:f>'Finance Discounts'!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{90C87B8F-2BAE-4B12-B68A-B2CC68DE8871}">
+          <x14:formula1>
+            <xm:f>'Transaction Discounts'!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7413B34F-E4AA-4DE3-84A0-AA3F404F6E52}">
+          <x14:formula1>
+            <xm:f>Phones!$C:$C</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AA5F0E8A-D26C-41ED-9017-5329724E19DE}">
+          <x14:formula1>
+            <xm:f>Phones!$B:$B</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AA3A71C4-39E0-44C2-B7B2-91D14287D908}">
+          <x14:formula1>
+            <xm:f>Phones!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A2A42168-92D7-4834-8A8D-90C71BF31288}">
+          <x14:formula1>
+            <xm:f>'Tariff Discounts'!$A$5:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{448D3AC8-3195-45E0-8B1D-3EDC4E0D7D7C}">
+          <x14:formula1>
+            <xm:f>Phones!D:D</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:F4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{07BAEEEF-CCDC-4F54-876D-E8F5079859D2}">
+          <x14:formula1>
+            <xm:f>Phones!F:F</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G4</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FBFF70-670B-4A58-881A-0F49E696B056}">
+  <sheetPr codeName="Sheet3">
+    <tabColor rgb="FFFF0066"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>-20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9632F243-C412-4B44-88D3-B90CF6289893}">
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFF0066"/>
@@ -770,7 +1113,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,88 +1163,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5FBFF70-670B-4A58-881A-0F49E696B056}">
-  <sheetPr codeName="Sheet3">
-    <tabColor rgb="FFFF0066"/>
-  </sheetPr>
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3">
-        <v>-150</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4">
-        <v>-560</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84E89506-491B-4CA4-9C30-76BE72E30CB7}">
   <sheetPr>
     <tabColor rgb="FFFF0066"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +1197,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -935,9 +1205,17 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
     </row>
@@ -949,7 +1227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27D0266-B495-4387-A906-19EDEB24C985}">
   <sheetPr codeName="Sheet4">
     <tabColor rgb="FFFF0066"/>
@@ -957,7 +1235,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1300,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB996A80-ABF5-4AC1-A3BC-5EF3FFB22A77}">
   <sheetPr codeName="Sheet5">
     <tabColor rgb="FFFF0066"/>
@@ -1030,7 +1308,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,144 +1363,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B22AAE5-670B-4978-B895-98848E155129}">
-  <sheetPr codeName="Sheet6">
-    <tabColor theme="0" tint="-0.499984740745262"/>
-  </sheetPr>
-  <dimension ref="A1:N1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1DB05AF6-9FA4-4C89-BAA8-0A780587DFAE}">
-          <x14:formula1>
-            <xm:f>'Commitment Discounts'!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{010B4CC7-6379-4402-8C78-E7F895B2AE00}">
-          <x14:formula1>
-            <xm:f>'Channel Discounts'!$A$2:$A$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7934C4F0-C7BC-4AC3-9AB6-528691B9406E}">
-          <x14:formula1>
-            <xm:f>'Finance Discounts'!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>K2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5700CBBF-8461-465E-99E8-1E6C38DF5C2F}">
-          <x14:formula1>
-            <xm:f>'Tariff Discounts'!$A$2:$A$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9811E644-9ECA-4ED8-97F4-88121B772C3A}">
-          <x14:formula1>
-            <xm:f>'Transaction Discounts'!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>J2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{49405E96-4A2D-41B5-93F5-B53F7F970734}">
-          <x14:formula1>
-            <xm:f>Phones!$C:$C</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9FAA79D8-36E8-4F82-8CC4-5C79D05EA1CA}">
-          <x14:formula1>
-            <xm:f>Phones!$B:$B</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5F8AB82E-12A9-453E-A74B-C5439C13BA15}">
-          <x14:formula1>
-            <xm:f>Phones!$A:$A</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B0593525-161D-43B5-9B9D-D6164033BEF5}">
-          <x14:formula1>
-            <xm:f>Phones!D:D</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:F2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>